<commit_message>
Added best dredge.v1 and m13 together to form a new column in TblS10
</commit_message>
<xml_diff>
--- a/results/TblS10.xlsx
+++ b/results/TblS10.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\CRI\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE14C99-6EB5-4466-B95B-59EF6878790F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TblS11_dredge" sheetId="1" r:id="rId1"/>
+    <sheet name="TblS10" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
-  <si>
-    <t>Estimates</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
+  <si>
+    <t>Predictors</t>
   </si>
   <si>
     <t>(Intercept)</t>
@@ -30,25 +31,61 @@
     <t>Jobs</t>
   </si>
   <si>
-    <t>-0.013 *</t>
+    <t>IncDiff</t>
+  </si>
+  <si>
+    <t>-0.012 *</t>
   </si>
   <si>
     <t>-0.025 ***</t>
   </si>
   <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>0.012 *</t>
+  </si>
+  <si>
     <t>0.014 *</t>
   </si>
   <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>-0.011 *</t>
+    <t>0.015 **</t>
+  </si>
+  <si>
+    <t>0.017 *</t>
+  </si>
+  <si>
+    <t>-0.019 **</t>
+  </si>
+  <si>
+    <t>-0.020 **</t>
   </si>
   <si>
     <t>0.048 ***</t>
   </si>
   <si>
-    <t>0.019 *</t>
+    <t>0.045 ***</t>
+  </si>
+  <si>
+    <t>0.043 ***</t>
+  </si>
+  <si>
+    <t>0.044 ***</t>
+  </si>
+  <si>
+    <t>0.018 *</t>
+  </si>
+  <si>
+    <t>0.020 *</t>
+  </si>
+  <si>
+    <t>0.027 *</t>
+  </si>
+  <si>
+    <t>0.025 *</t>
+  </si>
+  <si>
+    <t>0.026 *</t>
   </si>
   <si>
     <t>IncDiff * Stock</t>
@@ -57,7 +94,16 @@
     <t>0.026 **</t>
   </si>
   <si>
-    <t>Jobs * twowayfe</t>
+    <t>0.025 **</t>
+  </si>
+  <si>
+    <t>Jobs * Stock</t>
+  </si>
+  <si>
+    <t>Unemp</t>
+  </si>
+  <si>
+    <t>Residual Variance</t>
   </si>
   <si>
     <t>Team-Level</t>
@@ -69,64 +115,155 @@
     <t>Total</t>
   </si>
   <si>
+    <t>Explained Variance</t>
+  </si>
+  <si>
     <t>AIC</t>
   </si>
   <si>
     <t>log-Likelihood</t>
   </si>
   <si>
-    <t>* p&lt;0.05   ** p&lt;0.01   *** p&lt;0.001</t>
-  </si>
-  <si>
-    <t>Income-Differences</t>
-  </si>
-  <si>
-    <t>Housing</t>
-  </si>
-  <si>
-    <t>Dependent Variable</t>
-  </si>
-  <si>
-    <t>Test Variable</t>
+    <t>Auto_1</t>
+  </si>
+  <si>
+    <t>Auto_2</t>
+  </si>
+  <si>
+    <t>Auto_3</t>
+  </si>
+  <si>
+    <t>Auto_4</t>
+  </si>
+  <si>
+    <t>Auto_5</t>
+  </si>
+  <si>
+    <t>m13 (Tbl S5)</t>
+  </si>
+  <si>
+    <t>DV (ref = all others)</t>
+  </si>
+  <si>
+    <t>Estimation (ref = all others)</t>
+  </si>
+  <si>
+    <t>Logit</t>
+  </si>
+  <si>
+    <t>OLS</t>
+  </si>
+  <si>
+    <t>Main Test Measure (ref = Flow)</t>
+  </si>
+  <si>
+    <t>Test: Immigration Stock</t>
+  </si>
+  <si>
+    <t>Test: Change in Flow</t>
   </si>
   <si>
     <t>Sample Includes:</t>
   </si>
   <si>
+    <t>1996 Wave</t>
+  </si>
+  <si>
+    <t>2006 Wave</t>
+  </si>
+  <si>
+    <t>2016 Wave</t>
+  </si>
+  <si>
+    <t>2006*2016 Interaction</t>
+  </si>
+  <si>
+    <t>13 Rich Democracies</t>
+  </si>
+  <si>
+    <t>Eastern Europe</t>
+  </si>
+  <si>
+    <t>All Available Countries</t>
+  </si>
+  <si>
     <t>Model Design</t>
   </si>
   <si>
-    <t>Interactions</t>
-  </si>
-  <si>
-    <t>Variance Explained</t>
-  </si>
-  <si>
-    <t>Fit</t>
-  </si>
-  <si>
-    <t>Change in Flow</t>
-  </si>
-  <si>
-    <t>2016 Wave</t>
-  </si>
-  <si>
-    <t>13 Rich Democracies</t>
-  </si>
-  <si>
-    <t>Eastern Europe</t>
-  </si>
-  <si>
-    <t>"Two-Way Fixed-Effects"</t>
+    <t>Algorithm Probed Interactions</t>
+  </si>
+  <si>
+    <t>"Two-Way Fixed Effects"</t>
   </si>
   <si>
     <t>Country-Year Level</t>
+  </si>
+  <si>
+    <t>Model Score</t>
+  </si>
+  <si>
+    <t>Any Clustering</t>
+  </si>
+  <si>
+    <t>Unbalanced Panel</t>
+  </si>
+  <si>
+    <t>GDP as Indep. Variable</t>
+  </si>
+  <si>
+    <t>Conservatism as Indep. Variable</t>
+  </si>
+  <si>
+    <t>Jobs * "Two-Way Fixed.."</t>
+  </si>
+  <si>
+    <t>Stock * "Two-Way Fixed.."</t>
+  </si>
+  <si>
+    <t>Any Clustering * GDP</t>
+  </si>
+  <si>
+    <t>OLS * Unbalanced Pan.</t>
+  </si>
+  <si>
+    <t>Public Employment as Indep. Variable</t>
+  </si>
+  <si>
+    <t>Unemp * Public Emp.</t>
+  </si>
+  <si>
+    <t>1996 Wave * Conservatism</t>
+  </si>
+  <si>
+    <t>Team-Test Level</t>
+  </si>
+  <si>
+    <t>Confidence interval, does not cross zero at * 95%   ** 99%   *** 99.9%</t>
+  </si>
+  <si>
+    <t>Model Statistics</t>
+  </si>
+  <si>
+    <t>-0.024 ***</t>
+  </si>
+  <si>
+    <t>0.013 *</t>
+  </si>
+  <si>
+    <t>0.028 *</t>
+  </si>
+  <si>
+    <t>Auto_1_m13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,7 +326,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,19 +400,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
@@ -581,8 +719,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -590,9 +730,7 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -621,53 +759,61 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -743,7 +889,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -755,7 +901,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -802,6 +948,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -837,6 +1000,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -988,223 +1168,1098 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:B28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="30.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="2" customWidth="1"/>
+    <col min="5" max="8" width="8.85546875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>-8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="G3" s="3">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-0.01</v>
+      </c>
+      <c r="E5" s="3">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="3">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3">
+        <v>-1.6E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="G18" s="3">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="H18" s="3">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="3">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="3">
+        <v>-1.9E-2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3">
+        <v>-0.02</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C24" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E24" s="3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F24" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G24" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H24" s="3">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="E26" s="3">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13">
+        <v>-2E-3</v>
+      </c>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H36" s="3">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3">
+        <v>-2E-3</v>
+      </c>
+      <c r="D37" s="3">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>-2E-3</v>
+      </c>
+      <c r="F37" s="3">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="G37" s="3">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="H37" s="3">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="3">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3">
+        <v>-4.7E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3">
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B45" s="3">
+        <v>5.22E-4</v>
+      </c>
+      <c r="C45" s="3">
+        <v>5.4000000000000001E-4</v>
+      </c>
+      <c r="D45" s="3">
+        <v>4.9399999999999997E-4</v>
+      </c>
+      <c r="E45" s="3">
+        <v>5.7200000000000003E-4</v>
+      </c>
+      <c r="F45" s="3">
+        <v>5.4900000000000001E-4</v>
+      </c>
+      <c r="G45" s="3">
+        <v>5.5900000000000004E-4</v>
+      </c>
+      <c r="H45" s="3">
+        <v>5.7399999999999997E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2">
-        <v>-8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B46" s="3">
+        <v>4.7679999999999997E-3</v>
+      </c>
+      <c r="C46" s="3">
+        <v>4.7540000000000004E-3</v>
+      </c>
+      <c r="D46" s="3">
+        <v>4.7410000000000004E-3</v>
+      </c>
+      <c r="E46" s="3">
+        <v>4.7520000000000001E-3</v>
+      </c>
+      <c r="F46" s="3">
+        <v>4.7559999999999998E-3</v>
+      </c>
+      <c r="G46" s="3">
+        <v>4.7569999999999999E-3</v>
+      </c>
+      <c r="H46" s="3">
+        <v>4.7369999999999999E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="2">
-        <v>1.7000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B47" s="3">
+        <v>5.2900000000000004E-3</v>
+      </c>
+      <c r="C47" s="3">
+        <v>5.2940000000000001E-3</v>
+      </c>
+      <c r="D47" s="16">
+        <v>5.2350000000000001E-3</v>
+      </c>
+      <c r="E47" s="3">
+        <v>5.3239999999999997E-3</v>
+      </c>
+      <c r="F47" s="3">
+        <v>5.3049999999999998E-3</v>
+      </c>
+      <c r="G47" s="3">
+        <v>5.3160000000000004E-3</v>
+      </c>
+      <c r="H47" s="3">
+        <v>5.3109999999999997E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="2">
-        <v>1.2E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="D48" s="16"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="6">
+        <v>0.15125114732900899</v>
+      </c>
+      <c r="C49" s="6">
+        <v>0.12198394551276801</v>
+      </c>
+      <c r="D49" s="6">
+        <v>0.196777905709829</v>
+      </c>
+      <c r="E49" s="6">
+        <v>6.9953364506117499E-2</v>
+      </c>
+      <c r="F49" s="6">
+        <v>0.107350344604648</v>
+      </c>
+      <c r="G49" s="6">
+        <v>9.1090788040069301E-2</v>
+      </c>
+      <c r="H49" s="6">
+        <v>6.6701453193201907E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="6">
+        <v>2.3398649983320498E-2</v>
+      </c>
+      <c r="C50" s="6">
+        <v>2.6266187504342502E-2</v>
+      </c>
+      <c r="D50" s="6">
+        <v>2.89289009167202E-2</v>
+      </c>
+      <c r="E50" s="6">
+        <v>2.6675835721631399E-2</v>
+      </c>
+      <c r="F50" s="6">
+        <v>2.5856539287053702E-2</v>
+      </c>
+      <c r="G50" s="6">
+        <v>2.5651715178409199E-2</v>
+      </c>
+      <c r="H50" s="6">
+        <v>2.9748197351298002E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="7">
+        <v>3.7702540765799701E-2</v>
+      </c>
+      <c r="C51" s="7">
+        <v>3.6974905635944001E-2</v>
+      </c>
+      <c r="D51" s="7">
+        <v>4.7707523801316001E-2</v>
+      </c>
+      <c r="E51" s="7">
+        <v>3.1517642162026099E-2</v>
+      </c>
+      <c r="F51" s="7">
+        <v>3.4973909028840802E-2</v>
+      </c>
+      <c r="G51" s="7">
+        <v>3.2972912421737499E-2</v>
+      </c>
+      <c r="H51" s="7">
+        <v>3.3882456334057301E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="2">
+        <v>87</v>
+      </c>
+      <c r="C52" s="2">
+        <v>87</v>
+      </c>
+      <c r="D52" s="2">
+        <v>87</v>
+      </c>
+      <c r="E52" s="2">
+        <v>87</v>
+      </c>
+      <c r="F52" s="2">
+        <v>87</v>
+      </c>
+      <c r="G52" s="2">
+        <v>87</v>
+      </c>
+      <c r="H52" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="8">
+        <v>1253</v>
+      </c>
+      <c r="C53" s="8">
+        <v>1253</v>
+      </c>
+      <c r="D53" s="8">
+        <v>1253</v>
+      </c>
+      <c r="E53" s="8">
+        <v>1253</v>
+      </c>
+      <c r="F53" s="8">
+        <v>1253</v>
+      </c>
+      <c r="G53" s="8">
+        <v>1253</v>
+      </c>
+      <c r="H53" s="8">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="2">
-        <v>1.4E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B54" s="9">
+        <v>-2913.7629999999999</v>
+      </c>
+      <c r="C54" s="9">
+        <v>-2935.2330000000002</v>
+      </c>
+      <c r="D54" s="9">
+        <v>-2888.3420000000001</v>
+      </c>
+      <c r="E54" s="9">
+        <v>-2909.3510000000001</v>
+      </c>
+      <c r="F54" s="9">
+        <v>-2910.3690000000001</v>
+      </c>
+      <c r="G54" s="9">
+        <v>-2909.3969999999999</v>
+      </c>
+      <c r="H54" s="9">
+        <v>-2915.692</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1.2E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="2">
-        <v>26.332000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1.403</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="2">
-        <v>4.2130000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="2">
-        <v>-2948.482</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="11">
-        <v>1489.241</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="B55" s="12">
+        <v>1476.8810000000001</v>
+      </c>
+      <c r="C55" s="12">
+        <v>1484.617</v>
+      </c>
+      <c r="D55" s="12">
+        <v>1468.171</v>
+      </c>
+      <c r="E55" s="12">
+        <v>1474.6759999999999</v>
+      </c>
+      <c r="F55" s="12">
+        <v>1475.184</v>
+      </c>
+      <c r="G55" s="12">
+        <v>1474.6980000000001</v>
+      </c>
+      <c r="H55" s="12">
+        <v>1477.846</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D57" s="7"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D59" s="8"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D60" s="9"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D61" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>